<commit_message>
Deploly do dashboard com indicadores extras
</commit_message>
<xml_diff>
--- a/database-archives/registro-extracoes.xlsx
+++ b/database-archives/registro-extracoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davis\OneDrive\Repositórios\Moer\moer\database-archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5AB21B-1982-4F1D-9A90-0D7D5D285CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4B2C01-C06D-4420-86CF-4A8818E8B0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{7DB036DA-06AA-406C-9B46-5FF9DFED1C20}"/>
   </bookViews>
@@ -729,7 +729,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -854,10 +854,10 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L10" s="2"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L9" s="2"/>
     </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25"/>
@@ -910,7 +910,7 @@
           <x14:formula1>
             <xm:f>dim_metodo!$B$2:$B100</xm:f>
           </x14:formula1>
-          <xm:sqref>E1048573:E1048576 E2</xm:sqref>
+          <xm:sqref>E1048572:E1048576 E2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F72B0E3-D53D-41B4-AF48-C57589F66542}">
           <x14:formula1>
@@ -920,9 +920,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8113300C-203F-459E-8959-E26F8A970D09}">
           <x14:formula1>
-            <xm:f>dim_metodo!$B$2:$B104</xm:f>
+            <xm:f>dim_metodo!$B$2:$B105</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E1048572</xm:sqref>
+          <xm:sqref>E3:E1048571</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1139,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>